<commit_message>
Plannig is af voor nu
De planning is niet echt helemaal fair voor nu, maar dat fixen we in
post
</commit_message>
<xml_diff>
--- a/Asset Lists/Asset_List_Codes.xlsx
+++ b/Asset Lists/Asset_List_Codes.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\Gamelab_3\Asset Lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\GameLab 3 Mack\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Artists" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="174">
   <si>
     <t>Assetlist</t>
   </si>
@@ -213,9 +213,6 @@
     <t>WE_Sword_004</t>
   </si>
   <si>
-    <t>WE_Sword_005</t>
-  </si>
-  <si>
     <t>WE_Axe_001</t>
   </si>
   <si>
@@ -535,6 +532,21 @@
   </si>
   <si>
     <t>Voor vragen ga naar Zinedine</t>
+  </si>
+  <si>
+    <t>WE_Spear_003</t>
+  </si>
+  <si>
+    <t>WE_Spear_004</t>
+  </si>
+  <si>
+    <t>Anthony &amp; Carlo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roos</t>
+  </si>
+  <si>
+    <t>2DE_HUD_ShopMenu</t>
   </si>
 </sst>
 </file>
@@ -950,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,7 +1081,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="1"/>
@@ -1085,7 +1097,7 @@
     </row>
     <row r="13" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -1094,7 +1106,7 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E14" s="9"/>
     </row>
@@ -1103,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="9"/>
     </row>
@@ -1112,7 +1124,7 @@
         <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E16" s="9"/>
     </row>
@@ -1121,7 +1133,7 @@
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E17" s="9"/>
     </row>
@@ -1130,7 +1142,7 @@
         <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18" s="9"/>
     </row>
@@ -1139,307 +1151,308 @@
         <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>105</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
       </c>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D23" t="s">
-        <v>85</v>
+        <v>104</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>114</v>
-      </c>
-      <c r="D25" t="s">
-        <v>86</v>
+        <v>112</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" t="s">
-        <v>91</v>
+        <v>113</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="D30" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" t="s">
-        <v>84</v>
+        <v>54</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D33" t="s">
-        <v>85</v>
+        <v>55</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>140</v>
-      </c>
-      <c r="D42" t="s">
-        <v>88</v>
+        <v>44</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>45</v>
-      </c>
-      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="D44" t="s">
-        <v>87</v>
+        <v>45</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" t="s">
-        <v>88</v>
+        <v>46</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>141</v>
-      </c>
-      <c r="D46" t="s">
-        <v>88</v>
+        <v>47</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>142</v>
-      </c>
-      <c r="D47" t="s">
-        <v>88</v>
+        <v>140</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>143</v>
       </c>
-      <c r="D48" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>144</v>
-      </c>
-      <c r="D49" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>121</v>
-      </c>
-      <c r="D50" t="s">
-        <v>91</v>
+      <c r="D50" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
-      </c>
-      <c r="D53" t="s">
-        <v>91</v>
+        <v>155</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
         <v>90</v>
       </c>
-      <c r="D54" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>89</v>
+      </c>
+      <c r="D55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D57" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>134</v>
-      </c>
-      <c r="D58" t="s">
-        <v>116</v>
+        <v>57</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>135</v>
-      </c>
-      <c r="D59" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>134</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>160</v>
-      </c>
-      <c r="D63" t="s">
-        <v>86</v>
+        <v>48</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>137</v>
-      </c>
-      <c r="D64" t="s">
+        <v>159</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1448,495 +1461,511 @@
         <v>136</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D66" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>49</v>
-      </c>
-      <c r="D70" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A76" s="3" t="s">
+    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
+    <row r="79" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>58</v>
-      </c>
-      <c r="D79" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>59</v>
-      </c>
-      <c r="D80" t="s">
-        <v>84</v>
+        <v>58</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>60</v>
-      </c>
-      <c r="D81" t="s">
-        <v>84</v>
+        <v>59</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
-      </c>
-      <c r="D82" t="s">
-        <v>84</v>
+        <v>60</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>62</v>
-      </c>
-      <c r="D83" t="s">
-        <v>91</v>
+        <v>61</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D84" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>63</v>
-      </c>
-      <c r="D86" t="s">
-        <v>86</v>
+        <v>62</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>96</v>
-      </c>
-      <c r="D87" t="s">
-        <v>86</v>
+        <v>95</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
-      </c>
-      <c r="D88" t="s">
-        <v>86</v>
+        <v>96</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
-      </c>
-      <c r="D89" t="s">
-        <v>86</v>
+        <v>97</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D91" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>106</v>
-      </c>
-      <c r="D92" t="s">
-        <v>87</v>
+        <v>169</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>107</v>
-      </c>
-      <c r="D93" t="s">
-        <v>87</v>
+        <v>170</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>108</v>
-      </c>
-      <c r="D94" t="s">
-        <v>87</v>
+        <v>105</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>64</v>
+        <v>106</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>147</v>
-      </c>
-      <c r="D96" t="s">
-        <v>88</v>
+        <v>107</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>148</v>
-      </c>
-      <c r="D97" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>125</v>
-      </c>
-      <c r="D98" t="s">
-        <v>91</v>
+        <v>146</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>126</v>
-      </c>
-      <c r="D99" t="s">
-        <v>91</v>
+        <v>147</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D100" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D101" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D102" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D103" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>112</v>
-      </c>
-      <c r="D104" t="s">
-        <v>87</v>
+        <v>109</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>109</v>
-      </c>
-      <c r="D105" t="s">
-        <v>87</v>
+        <v>110</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>65</v>
+        <v>111</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>66</v>
+        <v>108</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>129</v>
-      </c>
-      <c r="D109" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>130</v>
-      </c>
-      <c r="D110" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D111" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="D112" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>151</v>
-      </c>
-      <c r="D113" t="s">
-        <v>88</v>
+        <v>149</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>161</v>
-      </c>
-      <c r="D114" t="s">
-        <v>84</v>
+        <v>148</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>162</v>
-      </c>
-      <c r="D115" t="s">
-        <v>84</v>
+        <v>150</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>163</v>
-      </c>
-      <c r="D116" t="s">
-        <v>84</v>
+        <v>160</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>115</v>
-      </c>
-      <c r="D117" t="s">
-        <v>116</v>
+        <v>161</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
-      </c>
-      <c r="D118" t="s">
-        <v>116</v>
+        <v>162</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
-      </c>
-      <c r="D119" t="s">
+        <v>114</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A121" s="3" t="s">
+      <c r="D120" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>117</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A123" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D121" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="E121" s="13"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>164</v>
-      </c>
-      <c r="D122" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>165</v>
-      </c>
-      <c r="D123" t="s">
-        <v>84</v>
-      </c>
+      <c r="D123" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E123" s="13"/>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>166</v>
-      </c>
-      <c r="D124" t="s">
-        <v>84</v>
+        <v>163</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>138</v>
-      </c>
-      <c r="D125" t="s">
-        <v>85</v>
+        <v>164</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>139</v>
-      </c>
-      <c r="D126" t="s">
-        <v>85</v>
+        <v>165</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="D127" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="D128" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>167</v>
-      </c>
-      <c r="D129" t="s">
-        <v>84</v>
+        <v>153</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>168</v>
-      </c>
-      <c r="D130" t="s">
-        <v>84</v>
+        <v>154</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>152</v>
-      </c>
-      <c r="D131" t="s">
-        <v>88</v>
+        <v>166</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>153</v>
-      </c>
-      <c r="D132" t="s">
-        <v>88</v>
+        <v>167</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>157</v>
-      </c>
-      <c r="D133" t="s">
-        <v>88</v>
+        <v>151</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>158</v>
-      </c>
-      <c r="D134" t="s">
-        <v>88</v>
+        <v>152</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>156</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>157</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1949,8 +1978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,7 +1991,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1971,7 +2000,7 @@
       </c>
       <c r="B2" s="5"/>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1980,7 +2009,7 @@
       </c>
       <c r="B3" s="5"/>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1989,7 +2018,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1998,43 +2027,43 @@
       </c>
       <c r="B5" s="5"/>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2043,7 +2072,7 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2052,7 +2081,7 @@
       </c>
       <c r="B11" s="5"/>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2061,70 +2090,70 @@
       </c>
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="5"/>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="5"/>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2133,7 +2162,7 @@
       </c>
       <c r="B20" s="5"/>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -2142,7 +2171,7 @@
       </c>
       <c r="B21" s="5"/>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2151,16 +2180,16 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2198,7 @@
       </c>
       <c r="B24" s="5"/>
       <c r="C24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -2178,7 +2207,7 @@
       </c>
       <c r="B25" s="5"/>
       <c r="C25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2187,7 +2216,7 @@
       </c>
       <c r="B26" s="5"/>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -2196,7 +2225,7 @@
       </c>
       <c r="B27" s="5"/>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -2205,7 +2234,7 @@
       </c>
       <c r="B28" s="5"/>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -2214,25 +2243,25 @@
       </c>
       <c r="B29" s="5"/>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Planning en Assetlist geupdated
Planing niet helemaal af. Moet nog kijken waar of we ook buffs erin gaan
stoppen en van zulk soort andere kleine dingetjes. Ga ik morgen wel over
hebben
</commit_message>
<xml_diff>
--- a/Asset Lists/Asset_List_Codes.xlsx
+++ b/Asset Lists/Asset_List_Codes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\GameLab 3 Mack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deltion\Derde Jaar\Gamelab_3\Asset Lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="158">
   <si>
     <t>Assetlist</t>
   </si>
@@ -447,12 +447,6 @@
     <t>LE_Arena_001</t>
   </si>
   <si>
-    <t>Bu_Destructible_001</t>
-  </si>
-  <si>
-    <t>EN_GitGudChest_001</t>
-  </si>
-  <si>
     <t>2DE_Achievements</t>
   </si>
   <si>
@@ -478,6 +472,33 @@
   </si>
   <si>
     <t>NP_Demonic_003</t>
+  </si>
+  <si>
+    <t>Michiel/Anthony</t>
+  </si>
+  <si>
+    <t>Kevin of iemand anders</t>
+  </si>
+  <si>
+    <t>moet nog even besproken worden</t>
+  </si>
+  <si>
+    <t>Michiel (gaan we buffs erin houden? Vraag aan zine of iemand anders)</t>
+  </si>
+  <si>
+    <t>PR_GitGudChest_001</t>
+  </si>
+  <si>
+    <t>PR_Shop_001</t>
+  </si>
+  <si>
+    <t>PR_Shop_002</t>
+  </si>
+  <si>
+    <t>BU_Destructible_001</t>
+  </si>
+  <si>
+    <t>BU_ControlPoint_001</t>
   </si>
 </sst>
 </file>
@@ -536,7 +557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -597,12 +618,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -616,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -633,7 +648,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -914,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1173,7 @@
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="15" t="s">
         <v>138</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1171,7 +1185,7 @@
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1183,20 +1197,20 @@
       <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
-        <v>147</v>
+      <c r="A24" s="15" t="s">
+        <v>145</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>132</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="16" t="s">
-        <v>142</v>
+      <c r="A25" s="15" t="s">
+        <v>140</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>133</v>
@@ -1207,8 +1221,8 @@
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="16" t="s">
-        <v>143</v>
+      <c r="A26" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>133</v>
@@ -1219,8 +1233,8 @@
       <c r="E26" s="9"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="16" t="s">
-        <v>144</v>
+      <c r="A27" s="15" t="s">
+        <v>142</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>133</v>
@@ -1231,8 +1245,8 @@
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="16" t="s">
-        <v>145</v>
+      <c r="A28" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>133</v>
@@ -1287,11 +1301,11 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>133</v>
+      <c r="B34" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>68</v>
@@ -1326,7 +1340,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>133</v>
@@ -1336,7 +1350,15 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
+      <c r="A40" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
@@ -1371,8 +1393,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>148</v>
+      <c r="A47" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>131</v>
@@ -1382,19 +1404,19 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>149</v>
+      <c r="A48" s="15" t="s">
+        <v>147</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>132</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>70</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>150</v>
+      <c r="A49" s="15" t="s">
+        <v>148</v>
       </c>
       <c r="B49" s="5" t="s">
         <v>132</v>
@@ -1465,7 +1487,7 @@
         <v>133</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,7 +1498,7 @@
         <v>133</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.35">
@@ -1502,7 +1524,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>131</v>
@@ -1511,36 +1533,36 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B68" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B69" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B70" s="14" t="s">
         <v>131</v>
@@ -1551,40 +1573,40 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B71" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B72" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="15" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="B73" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>131</v>
@@ -1595,7 +1617,7 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" s="14" t="s">
         <v>131</v>
@@ -1606,76 +1628,76 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="15" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B76" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D76" t="s">
-        <v>71</v>
+      <c r="D76" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="15" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B77" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D77" t="s">
-        <v>71</v>
+      <c r="D77" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="15" t="s">
-        <v>126</v>
+        <v>72</v>
       </c>
       <c r="B78" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>66</v>
+      <c r="D78" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="15" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="B79" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>66</v>
+      <c r="D79" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="15" t="s">
-        <v>85</v>
+        <v>126</v>
       </c>
       <c r="B80" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B81" s="7" t="s">
-        <v>133</v>
+        <v>127</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>132</v>
+        <v>85</v>
+      </c>
+      <c r="B82" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>69</v>
@@ -1683,10 +1705,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" s="14" t="s">
-        <v>131</v>
+        <v>86</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>69</v>
@@ -1694,10 +1716,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="B84" s="14" t="s">
-        <v>131</v>
+        <v>87</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>69</v>
@@ -1705,29 +1727,29 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="15" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B85" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D85" t="s">
-        <v>71</v>
+      <c r="D85" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B86" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D86" t="s">
-        <v>71</v>
+      <c r="D86" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B87" s="14" t="s">
         <v>131</v>
@@ -1738,7 +1760,7 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B88" s="14" t="s">
         <v>131</v>
@@ -1749,32 +1771,32 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>69</v>
+        <v>102</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D89" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>69</v>
+        <v>103</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D90" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B91" s="5" t="s">
-        <v>132</v>
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>69</v>
@@ -1782,10 +1804,10 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B92" s="5" t="s">
-        <v>132</v>
+        <v>90</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>69</v>
@@ -1793,54 +1815,54 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B93" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D93" t="s">
-        <v>71</v>
+        <v>91</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D94" t="s">
-        <v>71</v>
+        <v>88</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>66</v>
+      <c r="D95" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B96" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D96" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>133</v>
+        <v>119</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>66</v>
@@ -1848,74 +1870,74 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="15" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>131</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>133</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B100" s="7" t="s">
-        <v>133</v>
+        <v>94</v>
+      </c>
+      <c r="B100" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A102" s="3" t="s">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D102" s="13" t="s">
+      <c r="D104" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="E102" s="13"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="B104" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>66</v>
-      </c>
+      <c r="E104" s="13"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>132</v>
+        <v>122</v>
+      </c>
+      <c r="B105" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>66</v>
@@ -1923,46 +1945,71 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D106" t="s">
-        <v>67</v>
+        <v>123</v>
+      </c>
+      <c r="B106" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B107" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D107" t="s">
-        <v>67</v>
+        <v>124</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B108" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>71</v>
+        <v>109</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D108" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="D109" s="1" t="s">
-        <v>69</v>
+      <c r="D109" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B110" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E111" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>